<commit_message>
add id in tab
</commit_message>
<xml_diff>
--- a/tabPanelBlock.xlsx
+++ b/tabPanelBlock.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mainhi/Documents/back/BaseDeDonneesViews/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621DE9CE-9667-924B-85B8-7B6F212B9ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED9E027-5915-524F-8417-B58264D0AE6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59180" yWindow="-13000" windowWidth="26420" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="67640" yWindow="-12660" windowWidth="26420" windowHeight="17200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Client" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="174">
   <si>
     <t>NameType</t>
   </si>
@@ -539,6 +539,9 @@
   </si>
   <si>
     <t>Ratio fabricant Pointes pour cloueur en unité par M131</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -568,21 +571,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -605,31 +602,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-9.9917600024414813E-2"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-9.9917600024414813E-2"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-9.9917600024414813E-2"/>
-      </top>
-      <bottom style="thin">
-        <color theme="2" tint="-9.9917600024414813E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -970,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:EM9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="EJ1" workbookViewId="0">
-      <selection activeCell="EO3" sqref="EO3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4042,7 +4023,432 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="R9" s="2"/>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9">
+        <v>9</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="M9">
+        <v>11</v>
+      </c>
+      <c r="N9">
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <v>13</v>
+      </c>
+      <c r="P9">
+        <v>14</v>
+      </c>
+      <c r="Q9">
+        <v>15</v>
+      </c>
+      <c r="R9">
+        <v>16</v>
+      </c>
+      <c r="S9">
+        <v>17</v>
+      </c>
+      <c r="T9">
+        <v>18</v>
+      </c>
+      <c r="U9">
+        <v>19</v>
+      </c>
+      <c r="V9">
+        <v>20</v>
+      </c>
+      <c r="W9">
+        <v>21</v>
+      </c>
+      <c r="X9">
+        <v>22</v>
+      </c>
+      <c r="Y9">
+        <v>23</v>
+      </c>
+      <c r="Z9">
+        <v>24</v>
+      </c>
+      <c r="AA9">
+        <v>25</v>
+      </c>
+      <c r="AB9">
+        <v>26</v>
+      </c>
+      <c r="AC9">
+        <v>27</v>
+      </c>
+      <c r="AD9">
+        <v>28</v>
+      </c>
+      <c r="AE9">
+        <v>29</v>
+      </c>
+      <c r="AF9">
+        <v>30</v>
+      </c>
+      <c r="AG9">
+        <v>31</v>
+      </c>
+      <c r="AH9">
+        <v>32</v>
+      </c>
+      <c r="AI9">
+        <v>33</v>
+      </c>
+      <c r="AJ9">
+        <v>34</v>
+      </c>
+      <c r="AK9">
+        <v>35</v>
+      </c>
+      <c r="AL9">
+        <v>36</v>
+      </c>
+      <c r="AM9">
+        <v>37</v>
+      </c>
+      <c r="AN9">
+        <v>38</v>
+      </c>
+      <c r="AO9">
+        <v>39</v>
+      </c>
+      <c r="AP9">
+        <v>40</v>
+      </c>
+      <c r="AQ9">
+        <v>41</v>
+      </c>
+      <c r="AR9">
+        <v>42</v>
+      </c>
+      <c r="AS9">
+        <v>43</v>
+      </c>
+      <c r="AT9">
+        <v>44</v>
+      </c>
+      <c r="AU9">
+        <v>45</v>
+      </c>
+      <c r="AV9">
+        <v>46</v>
+      </c>
+      <c r="AW9">
+        <v>47</v>
+      </c>
+      <c r="AX9">
+        <v>48</v>
+      </c>
+      <c r="AY9">
+        <v>49</v>
+      </c>
+      <c r="AZ9">
+        <v>50</v>
+      </c>
+      <c r="BA9">
+        <v>51</v>
+      </c>
+      <c r="BB9">
+        <v>52</v>
+      </c>
+      <c r="BC9">
+        <v>53</v>
+      </c>
+      <c r="BD9">
+        <v>54</v>
+      </c>
+      <c r="BE9">
+        <v>55</v>
+      </c>
+      <c r="BF9">
+        <v>56</v>
+      </c>
+      <c r="BG9">
+        <v>57</v>
+      </c>
+      <c r="BH9">
+        <v>58</v>
+      </c>
+      <c r="BI9">
+        <v>59</v>
+      </c>
+      <c r="BJ9">
+        <v>60</v>
+      </c>
+      <c r="BK9">
+        <v>61</v>
+      </c>
+      <c r="BL9">
+        <v>62</v>
+      </c>
+      <c r="BM9">
+        <v>63</v>
+      </c>
+      <c r="BN9">
+        <v>64</v>
+      </c>
+      <c r="BO9">
+        <v>65</v>
+      </c>
+      <c r="BP9">
+        <v>66</v>
+      </c>
+      <c r="BQ9">
+        <v>67</v>
+      </c>
+      <c r="BR9">
+        <v>68</v>
+      </c>
+      <c r="BS9">
+        <v>69</v>
+      </c>
+      <c r="BT9">
+        <v>70</v>
+      </c>
+      <c r="BU9">
+        <v>71</v>
+      </c>
+      <c r="BV9">
+        <v>72</v>
+      </c>
+      <c r="BW9">
+        <v>73</v>
+      </c>
+      <c r="BX9">
+        <v>74</v>
+      </c>
+      <c r="BY9">
+        <v>75</v>
+      </c>
+      <c r="BZ9">
+        <v>76</v>
+      </c>
+      <c r="CA9">
+        <v>77</v>
+      </c>
+      <c r="CB9">
+        <v>78</v>
+      </c>
+      <c r="CC9">
+        <v>79</v>
+      </c>
+      <c r="CD9">
+        <v>80</v>
+      </c>
+      <c r="CE9">
+        <v>81</v>
+      </c>
+      <c r="CF9">
+        <v>82</v>
+      </c>
+      <c r="CG9">
+        <v>83</v>
+      </c>
+      <c r="CH9">
+        <v>84</v>
+      </c>
+      <c r="CI9">
+        <v>85</v>
+      </c>
+      <c r="CJ9">
+        <v>86</v>
+      </c>
+      <c r="CK9">
+        <v>87</v>
+      </c>
+      <c r="CL9">
+        <v>88</v>
+      </c>
+      <c r="CM9">
+        <v>89</v>
+      </c>
+      <c r="CN9">
+        <v>90</v>
+      </c>
+      <c r="CO9">
+        <v>91</v>
+      </c>
+      <c r="CP9">
+        <v>92</v>
+      </c>
+      <c r="CQ9">
+        <v>93</v>
+      </c>
+      <c r="CR9">
+        <v>94</v>
+      </c>
+      <c r="CS9">
+        <v>95</v>
+      </c>
+      <c r="CT9">
+        <v>96</v>
+      </c>
+      <c r="CU9">
+        <v>97</v>
+      </c>
+      <c r="CV9">
+        <v>98</v>
+      </c>
+      <c r="CW9">
+        <v>99</v>
+      </c>
+      <c r="CX9">
+        <v>100</v>
+      </c>
+      <c r="CY9">
+        <v>101</v>
+      </c>
+      <c r="CZ9">
+        <v>102</v>
+      </c>
+      <c r="DA9">
+        <v>103</v>
+      </c>
+      <c r="DB9">
+        <v>104</v>
+      </c>
+      <c r="DC9">
+        <v>105</v>
+      </c>
+      <c r="DD9">
+        <v>106</v>
+      </c>
+      <c r="DE9">
+        <v>107</v>
+      </c>
+      <c r="DF9">
+        <v>108</v>
+      </c>
+      <c r="DG9">
+        <v>109</v>
+      </c>
+      <c r="DH9">
+        <v>110</v>
+      </c>
+      <c r="DI9">
+        <v>111</v>
+      </c>
+      <c r="DJ9">
+        <v>112</v>
+      </c>
+      <c r="DK9">
+        <v>113</v>
+      </c>
+      <c r="DL9">
+        <v>114</v>
+      </c>
+      <c r="DM9">
+        <v>115</v>
+      </c>
+      <c r="DN9">
+        <v>116</v>
+      </c>
+      <c r="DO9">
+        <v>117</v>
+      </c>
+      <c r="DP9">
+        <v>118</v>
+      </c>
+      <c r="DQ9">
+        <v>119</v>
+      </c>
+      <c r="DR9">
+        <v>120</v>
+      </c>
+      <c r="DS9">
+        <v>121</v>
+      </c>
+      <c r="DT9">
+        <v>122</v>
+      </c>
+      <c r="DU9">
+        <v>123</v>
+      </c>
+      <c r="DV9">
+        <v>124</v>
+      </c>
+      <c r="DW9">
+        <v>125</v>
+      </c>
+      <c r="DX9">
+        <v>126</v>
+      </c>
+      <c r="DY9">
+        <v>127</v>
+      </c>
+      <c r="DZ9">
+        <v>128</v>
+      </c>
+      <c r="EA9">
+        <v>129</v>
+      </c>
+      <c r="EB9">
+        <v>130</v>
+      </c>
+      <c r="EC9">
+        <v>131</v>
+      </c>
+      <c r="ED9">
+        <v>132</v>
+      </c>
+      <c r="EE9">
+        <v>133</v>
+      </c>
+      <c r="EF9">
+        <v>134</v>
+      </c>
+      <c r="EG9">
+        <v>135</v>
+      </c>
+      <c r="EH9">
+        <v>136</v>
+      </c>
+      <c r="EI9">
+        <v>137</v>
+      </c>
+      <c r="EJ9">
+        <v>138</v>
+      </c>
+      <c r="EK9">
+        <v>139</v>
+      </c>
+      <c r="EL9">
+        <v>140</v>
+      </c>
+      <c r="EM9">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>